<commit_message>
Essai correction mapping Medication b1dcc1472ac62410e9e3991c96b69680ec2b7a49
</commit_message>
<xml_diff>
--- a/MappingPosologie/ig/PN13-FHIR-prescmed-dosageinstruction-conceptmap.xlsx
+++ b/MappingPosologie/ig/PN13-FHIR-prescmed-dosageinstruction-conceptmap.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-11-13T17:25:07+00:00</t>
+    <t>2024-11-16T17:09:48+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>Dosage.timing.periodUnit</t>
+  </si>
+  <si>
+    <t>Elément_posologie</t>
+  </si>
+  <si>
+    <t>Dosage.timing</t>
   </si>
 </sst>
 </file>
@@ -399,7 +405,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -478,6 +484,19 @@
       </c>
       <c r="E5" s="2"/>
     </row>
+    <row r="6">
+      <c r="A6" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
mise a jour mapping posologie pour reunion ef2bdf36d95fd7302ceb15e853eb11298b18e179
</commit_message>
<xml_diff>
--- a/MappingPosologie/ig/PN13-FHIR-prescmed-dosageinstruction-conceptmap.xlsx
+++ b/MappingPosologie/ig/PN13-FHIR-prescmed-dosageinstruction-conceptmap.xlsx
@@ -10,12 +10,13 @@
     <sheet name="Mapping Table 0" r:id="rId4" sheetId="2"/>
     <sheet name="Mapping Table 1" r:id="rId5" sheetId="3"/>
     <sheet name="Mapping Table 2" r:id="rId6" sheetId="4"/>
+    <sheet name="Mapping Table 3" r:id="rId7" sheetId="5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="51">
   <si>
     <t>Property</t>
   </si>
@@ -59,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-11-17T16:50:27+00:00</t>
+    <t>2024-11-18T17:53:13+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -156,6 +157,18 @@
   </si>
   <si>
     <t>Dosage.timing.repeat.dayOfWeek</t>
+  </si>
+  <si>
+    <t>Elément_posologie/Quantité/Nombre</t>
+  </si>
+  <si>
+    <t>Dosage.doseAndRate.doseQuantity.value</t>
+  </si>
+  <si>
+    <t>Elément_posologie/Quantité/Unité</t>
+  </si>
+  <si>
+    <t>Dosage.doseAndRate.doseQuantity.unité</t>
   </si>
 </sst>
 </file>
@@ -709,6 +722,140 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s" s="1">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2"/>
+      <c r="B2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D7" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D8" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -747,27 +894,27 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
         <v>39</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E4" s="2"/>
     </row>

</xml_diff>